<commit_message>
Did few changes in Data
</commit_message>
<xml_diff>
--- a/Data/BOD.xlsx
+++ b/Data/BOD.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaidehi Mishra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Acad stuff\SEM VII\HS4870\project\Modelling and report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AC1FDC-EE45-4530-A7A2-74BD52ABD0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2856" windowWidth="17280" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOD" sheetId="1" r:id="rId1"/>
+    <sheet name="Averaged" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Min</t>
   </si>
@@ -77,12 +77,18 @@
   </si>
   <si>
     <t xml:space="preserve">BOD River Wise Data (Unit: mg/L) </t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>BOD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -169,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,13 +203,19 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,11 +497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,27 +511,35 @@
     <col min="16" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12">
@@ -550,9 +570,25 @@
         <v>2011</v>
       </c>
       <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="P2" s="12">
+        <v>2010</v>
+      </c>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12">
+        <v>2009</v>
+      </c>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12">
+        <v>2008</v>
+      </c>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12">
+        <v>2007</v>
+      </c>
+      <c r="W2" s="12"/>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,8 +631,32 @@
       <c r="O3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -642,8 +702,32 @@
       <c r="O4" s="7">
         <v>4.3272727272727272</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="7">
+        <v>1.1333333333333331</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4.5333333333333332</v>
+      </c>
+      <c r="R4" s="7">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="S4" s="7">
+        <v>7.5238095238095237</v>
+      </c>
+      <c r="T4" s="7">
+        <v>1.48</v>
+      </c>
+      <c r="U4" s="7">
+        <v>4.6850000000000005</v>
+      </c>
+      <c r="V4" s="7">
+        <v>1.1285714285714286</v>
+      </c>
+      <c r="W4" s="7">
+        <v>3.2714285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -685,8 +769,32 @@
       <c r="O5" s="7">
         <v>0.74782608695652175</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="7">
+        <v>0.36521739130434777</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>0.90869565217391324</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0.43500000000000005</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0.98999999999999988</v>
+      </c>
+      <c r="T5" s="7">
+        <v>0.38421052631578945</v>
+      </c>
+      <c r="U5" s="7">
+        <v>1.236842105263158</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0.34210526315789469</v>
+      </c>
+      <c r="W5" s="7">
+        <v>0.95789473684210524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -732,8 +840,32 @@
       <c r="O6" s="1">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="1">
+        <v>2.17</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>4.22</v>
+      </c>
+      <c r="R6" s="7">
+        <v>2.130612244897959</v>
+      </c>
+      <c r="S6" s="7">
+        <v>3.6693877551020408</v>
+      </c>
+      <c r="T6" s="7">
+        <v>2.2054054054054051</v>
+      </c>
+      <c r="U6" s="7">
+        <v>4.4459459459459474</v>
+      </c>
+      <c r="V6" s="7">
+        <v>1.9105263157894739</v>
+      </c>
+      <c r="W6" s="7">
+        <v>3.7763157894736836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -779,8 +911,32 @@
       <c r="O7" s="1">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="7">
+        <v>2.2370370370370369</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>12.292592592592595</v>
+      </c>
+      <c r="R7" s="7">
+        <v>3.6913043478260872</v>
+      </c>
+      <c r="S7" s="7">
+        <v>15.430434782608694</v>
+      </c>
+      <c r="T7" s="7">
+        <v>4.339130434782609</v>
+      </c>
+      <c r="U7" s="7">
+        <v>15.921739130434782</v>
+      </c>
+      <c r="V7" s="7">
+        <v>2.4478260869565216</v>
+      </c>
+      <c r="W7" s="7">
+        <v>14.660869565217391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -826,8 +982,32 @@
       <c r="O8" s="7">
         <v>3.7700000000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>4.34</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="S8" s="7">
+        <v>4.22</v>
+      </c>
+      <c r="T8" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U8" s="7">
+        <v>3.13</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="W8" s="1">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -869,8 +1049,32 @@
       <c r="O9" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="R9" s="7">
+        <v>10.385714285714286</v>
+      </c>
+      <c r="S9" s="7">
+        <v>24.857142857142858</v>
+      </c>
+      <c r="T9" s="8">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="U9" s="8">
+        <v>16.111111111111111</v>
+      </c>
+      <c r="V9" s="7">
+        <v>72.875</v>
+      </c>
+      <c r="W9" s="7">
+        <v>74.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -916,8 +1120,32 @@
       <c r="O10" s="7">
         <v>2.677777777777778</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="8">
+        <v>0.98260869565217379</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>2.6434782608695655</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="S10" s="7">
+        <v>3.2652173913043483</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.82727272727272738</v>
+      </c>
+      <c r="U10" s="7">
+        <v>3.0909090909090917</v>
+      </c>
+      <c r="V10" s="7">
+        <v>1.8285714285714287</v>
+      </c>
+      <c r="W10" s="7">
+        <v>2.5214285714285714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -963,8 +1191,32 @@
       <c r="O11" s="1">
         <v>2.35</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>3.19</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0.80434782608695654</v>
+      </c>
+      <c r="S11" s="7">
+        <v>2.1130434782608698</v>
+      </c>
+      <c r="T11" s="7">
+        <v>1.0111111111111113</v>
+      </c>
+      <c r="U11" s="7">
+        <v>2.088888888888889</v>
+      </c>
+      <c r="V11" s="7">
+        <v>2.3777777777777782</v>
+      </c>
+      <c r="W11" s="7">
+        <v>2.3777777777777782</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1010,8 +1262,32 @@
       <c r="O12" s="7">
         <v>8.774285714285714</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="7">
+        <v>2.1685714285714282</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>8.8285714285714292</v>
+      </c>
+      <c r="R12" s="8">
+        <v>2.2029411764705884</v>
+      </c>
+      <c r="S12" s="8">
+        <v>6.8741176470588226</v>
+      </c>
+      <c r="T12" s="7">
+        <v>2.3323529411764703</v>
+      </c>
+      <c r="U12" s="7">
+        <v>5.9941176470588236</v>
+      </c>
+      <c r="V12" s="7">
+        <v>2.5272727272727273</v>
+      </c>
+      <c r="W12" s="7">
+        <v>8.5090909090909115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1057,8 +1333,32 @@
       <c r="O13" s="9">
         <v>5.4260869565217389</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="7">
+        <v>1.2913043478260868</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>4.5739130434782593</v>
+      </c>
+      <c r="R13" s="8">
+        <v>2.1045454545454541</v>
+      </c>
+      <c r="S13" s="8">
+        <v>5.1909090909090914</v>
+      </c>
+      <c r="T13" s="7">
+        <v>2.1272727272727274</v>
+      </c>
+      <c r="U13" s="7">
+        <v>5.6409090909090907</v>
+      </c>
+      <c r="V13" s="7">
+        <v>1.1157894736842107</v>
+      </c>
+      <c r="W13" s="7">
+        <v>3.9947368421052629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1104,10 +1404,84 @@
       <c r="O14" s="7">
         <v>2.8206896551724139</v>
       </c>
+      <c r="P14" s="7">
+        <v>0.57391304347826089</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>3.6347826086956525</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="S14" s="8">
+        <v>3.835</v>
+      </c>
+      <c r="T14" s="7">
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="U14" s="7">
+        <v>3.4899999999999998</v>
+      </c>
+      <c r="V14" s="7">
+        <v>0.56999999999999984</v>
+      </c>
+      <c r="W14" s="7">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B16" s="15">
+        <f xml:space="preserve"> AVERAGE(B4:C14)</f>
+        <v>6.4014813731680382</v>
+      </c>
+      <c r="D16" s="15">
+        <f xml:space="preserve"> AVERAGE(D4:E14)</f>
+        <v>5.3345621166569792</v>
+      </c>
+      <c r="F16" s="15">
+        <f xml:space="preserve"> AVERAGE(F4:G14)</f>
+        <v>3.8762361606850093</v>
+      </c>
+      <c r="H16" s="15">
+        <f xml:space="preserve"> AVERAGE(H4:I14)</f>
+        <v>3.3520579063146996</v>
+      </c>
+      <c r="J16" s="15">
+        <f xml:space="preserve"> AVERAGE(J4:K14)</f>
+        <v>4.3977947358965146</v>
+      </c>
+      <c r="L16" s="15">
+        <f xml:space="preserve"> AVERAGE(L4:M14)</f>
+        <v>3.8252474202686146</v>
+      </c>
+      <c r="N16" s="15">
+        <f xml:space="preserve"> AVERAGE(N4:O14)</f>
+        <v>3.8582941724729931</v>
+      </c>
+      <c r="P16" s="15">
+        <f xml:space="preserve"> AVERAGE(P4:Q14)</f>
+        <v>3.1166978271326098</v>
+      </c>
+      <c r="R16" s="15">
+        <f xml:space="preserve"> AVERAGE(R4:S14)</f>
+        <v>4.7538724785638289</v>
+      </c>
+      <c r="T16" s="15">
+        <f xml:space="preserve"> AVERAGE(T4:U14)</f>
+        <v>4.0432826765389871</v>
+      </c>
+      <c r="V16" s="15">
+        <f xml:space="preserve"> AVERAGE(V4:W14)</f>
+        <v>9.5144537847793487</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:O1"/>
+  <mergeCells count="13">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="A1:W1"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C2"/>
@@ -1119,4 +1493,105 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2017</v>
+      </c>
+      <c r="C1">
+        <f xml:space="preserve"> B1-1</f>
+        <v>2016</v>
+      </c>
+      <c r="D1">
+        <f t="shared" ref="D1:L1" si="0" xml:space="preserve"> C1-1</f>
+        <v>2015</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="F1">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>6.4014813731680382</v>
+      </c>
+      <c r="C2">
+        <v>5.3345621166569792</v>
+      </c>
+      <c r="D2">
+        <v>3.8762361606850093</v>
+      </c>
+      <c r="E2">
+        <v>3.3520579063146996</v>
+      </c>
+      <c r="F2">
+        <v>4.3977947358965146</v>
+      </c>
+      <c r="G2">
+        <v>3.8252474202686146</v>
+      </c>
+      <c r="H2">
+        <v>3.8582941724729931</v>
+      </c>
+      <c r="I2">
+        <v>3.1166978271326098</v>
+      </c>
+      <c r="J2">
+        <v>4.7538724785638289</v>
+      </c>
+      <c r="K2">
+        <v>4.0432826765389871</v>
+      </c>
+      <c r="L2">
+        <v>9.5144537847793487</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>